<commit_message>
DBs Dcumentacion e integracion sif 2023
</commit_message>
<xml_diff>
--- a/InformeFICsAbril2023.xlsx
+++ b/InformeFICsAbril2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bancolombia-my.sharepoint.com/personal/juliavar_bancolombia_com_co/Documents/Workspace/PruebaStreamLit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{E43D08A7-9A75-40E8-B59D-6AC8993F2F02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="280" documentId="14_{E43D08A7-9A75-40E8-B59D-6AC8993F2F02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7E96733-EB20-4559-AD7A-2123211632B8}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F3D96AE9-0F86-4742-BBBC-4A4B76F80A99}"/>
   </bookViews>
@@ -1009,8 +1009,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:Z281"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="G72" sqref="G72"/>
+    <sheetView tabSelected="1" topLeftCell="A261" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B281"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>